<commit_message>
Adding new CV mode class, updated segmentation ID for soccer field
</commit_message>
<xml_diff>
--- a/airsim_gd/dataset/levels_objects.xlsx
+++ b/airsim_gd/dataset/levels_objects.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15720" windowHeight="8115" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15720" windowHeight="8115"/>
   </bookViews>
   <sheets>
     <sheet name="Soccer_Field_Medium" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Building99_Hard!$A$1:$C$1914</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Soccer_Field_Medium!$A$1:$C$204</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ZhangJiaJie_Medium!$A$1:$C$1</definedName>
     <definedName name="soccer_zzz" localSheetId="1">ZhangJiaJie_Medium!$A$2:$B$1675</definedName>
   </definedNames>
@@ -11457,8 +11458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C204"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35:B36"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="B93" sqref="B93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12612,11 +12613,11 @@
         <v>46</v>
       </c>
       <c r="B96" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="C96">
         <f>VLOOKUP(Soccer_Field_Medium!B96,SegmentIDs!$A$2:$B$43,2, FALSE)</f>
-        <v>0</v>
+        <v>150</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -13916,6 +13917,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C204"/>
   <sortState ref="A2:A204">
     <sortCondition ref="A1"/>
   </sortState>
@@ -34046,8 +34048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1914"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Minor bug fixes, data generation chain fixes, nominal racer for dataset updated
</commit_message>
<xml_diff>
--- a/airsim_gd/dataset/levels_objects.xlsx
+++ b/airsim_gd/dataset/levels_objects.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tachy\Documents\Projects\Game_of_Drones\code\airsim_gd\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA8A2DB8-6C14-4306-BB13-72319F78D80F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24CA8EF3-F141-4054-ADAD-30E7A87409E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="1185" windowWidth="24240" windowHeight="13290" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7545" yWindow="4575" windowWidth="38700" windowHeight="15555" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Soccer_Field_Medium" sheetId="1" r:id="rId1"/>
@@ -28,12 +28,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -53,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7659" uniqueCount="3716">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7659" uniqueCount="3717">
   <si>
     <t>DefaultPhysicsVolume_0</t>
   </si>
@@ -11201,6 +11195,9 @@
   </si>
   <si>
     <t>notes</t>
+  </si>
+  <si>
+    <t>class</t>
   </si>
 </sst>
 </file>
@@ -57117,9 +57114,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -57130,7 +57125,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>203</v>
+        <v>3716</v>
       </c>
       <c r="B1" t="s">
         <v>232</v>

</xml_diff>